<commit_message>
gp files und notizen
</commit_message>
<xml_diff>
--- a/Korpus/korpusinfo.xlsx
+++ b/Korpus/korpusinfo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="2120" windowWidth="22260" windowHeight="12640"/>
+    <workbookView xWindow="2440" yWindow="2500" windowWidth="23740" windowHeight="12640"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -396,12 +396,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -416,12 +422,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -738,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1010,6 +1017,12 @@
       <c r="A16" t="s">
         <v>26</v>
       </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
       <c r="D16" t="s">
         <v>47</v>
       </c>
@@ -1021,6 +1034,12 @@
       <c r="A17" t="s">
         <v>27</v>
       </c>
+      <c r="B17">
+        <v>4.5</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
       <c r="D17" t="s">
         <v>47</v>
       </c>
@@ -1032,6 +1051,12 @@
       <c r="A18" t="s">
         <v>28</v>
       </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>30</v>
+      </c>
       <c r="D18" t="s">
         <v>47</v>
       </c>
@@ -1043,6 +1068,12 @@
       <c r="A19" t="s">
         <v>29</v>
       </c>
+      <c r="B19">
+        <v>4.5</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
       <c r="D19" t="s">
         <v>47</v>
       </c>
@@ -1054,6 +1085,9 @@
       <c r="A20" t="s">
         <v>31</v>
       </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
       <c r="D20" t="s">
         <v>47</v>
       </c>
@@ -1065,6 +1099,12 @@
       <c r="A21" t="s">
         <v>32</v>
       </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>13</v>
+      </c>
       <c r="D21" t="s">
         <v>47</v>
       </c>
@@ -1076,6 +1116,12 @@
       <c r="A22" t="s">
         <v>34</v>
       </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>9</v>
+      </c>
       <c r="D22" t="s">
         <v>47</v>
       </c>
@@ -1087,6 +1133,12 @@
       <c r="A23" t="s">
         <v>36</v>
       </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
       <c r="D23" t="s">
         <v>47</v>
       </c>
@@ -1098,6 +1150,12 @@
       <c r="A24" t="s">
         <v>38</v>
       </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
       <c r="D24" t="s">
         <v>47</v>
       </c>
@@ -1109,6 +1167,12 @@
       <c r="A25" t="s">
         <v>39</v>
       </c>
+      <c r="B25">
+        <v>4.5</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
       <c r="D25" t="s">
         <v>47</v>
       </c>
@@ -1117,8 +1181,11 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>41</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
       </c>
       <c r="D26" t="s">
         <v>47</v>
@@ -1131,6 +1198,12 @@
       <c r="A27" t="s">
         <v>42</v>
       </c>
+      <c r="B27">
+        <v>4.5</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
       <c r="D27" t="s">
         <v>47</v>
       </c>
@@ -1142,6 +1215,12 @@
       <c r="A28" t="s">
         <v>44</v>
       </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
       <c r="D28" t="s">
         <v>47</v>
       </c>
@@ -1152,6 +1231,12 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>45</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
       </c>
       <c r="D29" t="s">
         <v>47</v>

</xml_diff>